<commit_message>
HDU and update excel RTI in sheet
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\computer 3th first term\arch\Pipeline-Processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CED995-298A-4653-A00D-C92F32A250DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E7A950-BD38-4FB7-BF23-591C76B91A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
+    <workbookView xWindow="7248" yWindow="3096" windowWidth="14460" windowHeight="8964" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="97">
   <si>
     <t>op</t>
   </si>
@@ -321,6 +324,9 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>1110</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -446,7 +452,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,14 +768,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143EB804-9F5F-4231-9BD8-F64F4BEDFFE9}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.109375" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="10" customWidth="1"/>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="8" width="16.88671875" customWidth="1"/>
@@ -879,7 +884,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -945,7 +950,7 @@
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="10" t="s">
         <v>91</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -996,7 +1001,7 @@
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="10" t="s">
         <v>92</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1050,7 +1055,7 @@
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1122,7 +1127,7 @@
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>94</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1182,7 +1187,7 @@
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1236,7 +1241,7 @@
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1296,7 +1301,7 @@
       <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -2659,7 +2664,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D34" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
op code and function
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\computer 3th first term\arch\Pipeline-Processor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\Pipeline-Processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E7A950-BD38-4FB7-BF23-591C76B91A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EF6066-6FBC-4088-BEF8-D17538C79547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7248" yWindow="3096" windowWidth="14460" windowHeight="8964" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
+    <workbookView xWindow="6108" yWindow="1560" windowWidth="17280" windowHeight="8880" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="92">
   <si>
     <t>op</t>
   </si>
@@ -266,30 +263,6 @@
     <t>1001</t>
   </si>
   <si>
-    <t>000</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>011</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
     <t>1010</t>
   </si>
   <si>
@@ -327,13 +300,22 @@
   </si>
   <si>
     <t>1110</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>xxxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +331,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -434,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -452,6 +441,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143EB804-9F5F-4231-9BD8-F64F4BEDFFE9}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,19 +777,19 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -873,10 +863,10 @@
         <v>0.33749999999999997</v>
       </c>
       <c r="F2" s="12">
-        <v>0.16874999999999998</v>
+        <v>0.21111111111111111</v>
       </c>
       <c r="G2" s="12">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="H2" s="12"/>
     </row>
@@ -885,22 +875,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" t="s">
@@ -951,22 +941,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" t="s">
@@ -1002,22 +992,22 @@
         <v>7</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" t="s">
@@ -1056,22 +1046,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" t="s">
@@ -1128,22 +1118,22 @@
         <v>10</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" t="s">
@@ -1188,22 +1178,22 @@
         <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" t="s">
@@ -1242,22 +1232,22 @@
         <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" t="s">
@@ -1302,22 +1292,22 @@
         <v>13</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" t="s">
@@ -1360,13 +1350,13 @@
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C11" s="10"/>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1379,16 +1369,16 @@
         <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" t="s">
@@ -1433,16 +1423,16 @@
         <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" t="s">
@@ -1487,16 +1477,16 @@
         <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" t="s">
@@ -1541,16 +1531,16 @@
         <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" t="s">
@@ -1595,16 +1585,16 @@
         <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>77</v>
+        <v>77</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" t="s">
@@ -1649,16 +1639,16 @@
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" t="s">
@@ -1703,16 +1693,16 @@
         <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" t="s">
@@ -1752,13 +1742,13 @@
     <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C19" s="10"/>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -1771,16 +1761,16 @@
         <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" t="s">
@@ -1846,16 +1836,16 @@
         <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" t="s">
@@ -1919,13 +1909,13 @@
     <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C22" s="10"/>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -1975,13 +1965,13 @@
     <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C23" s="10"/>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -1994,16 +1984,16 @@
         <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" t="s">
@@ -2060,19 +2050,19 @@
         <v>23</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" t="s">
@@ -2135,19 +2125,19 @@
         <v>24</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" t="s">
@@ -2208,13 +2198,13 @@
     <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C27" s="10"/>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -2227,16 +2217,16 @@
         <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" t="s">
@@ -2304,16 +2294,16 @@
         <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="H29" s="10"/>
       <c r="I29" t="s">
@@ -2378,16 +2368,16 @@
         <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" t="s">
@@ -2452,16 +2442,16 @@
         <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" t="s">
@@ -2526,16 +2516,16 @@
         <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" t="s">
@@ -2595,19 +2585,19 @@
         <v>30</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" t="s">
@@ -2664,19 +2654,19 @@
         <v>31</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" t="s">
@@ -2726,19 +2716,11 @@
       </c>
       <c r="AC34">
         <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C35">
-        <v>1011</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
-      </c>
-      <c r="C36">
-        <v>1100</v>
       </c>
       <c r="I36" t="s">
         <v>8</v>

</xml_diff>